<commit_message>
Plot macro data and poliy rates EA + US
</commit_message>
<xml_diff>
--- a/Data/Attachments/Assignment_figures_CPI_rates.xlsx
+++ b/Data/Attachments/Assignment_figures_CPI_rates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A2010180\Dropbox\Penningpolitiken_2024\Task to PhD students\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stockholmuniversity-my.sharepoint.com/personal/edah1482_win_su_se/Documents/PhD/Year 2/Courses/Monetary/Assignments/RB Evaluation/cemof_evaluation/Data/Attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0941FC-9EBD-4806-B695-A81FBCA59AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{0877216D-C975-4A0B-9FDA-FB24FB78080E}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30220" windowHeight="17420" activeTab="1" xr2:uid="{0877216D-C975-4A0B-9FDA-FB24FB78080E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -273,7 +273,7 @@
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$61</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>43831</c:v>
@@ -684,7 +684,7 @@
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$61</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>43831</c:v>
@@ -1095,7 +1095,7 @@
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$61</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>43831</c:v>
@@ -1514,7 +1514,7 @@
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$61</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>43831</c:v>
@@ -1915,7 +1915,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2063,7 +2063,7 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2226,7 +2226,7 @@
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$61</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>43831</c:v>
@@ -2645,7 +2645,7 @@
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$61</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>43831</c:v>
@@ -3046,7 +3046,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3194,7 +3194,7 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3347,7 +3347,7 @@
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$61</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>43831</c:v>
@@ -3758,7 +3758,7 @@
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$61</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>43831</c:v>
@@ -4177,7 +4177,7 @@
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$61</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>43831</c:v>
@@ -4578,7 +4578,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4726,7 +4726,7 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4879,7 +4879,7 @@
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$61</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>43831</c:v>
@@ -5290,7 +5290,7 @@
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$61</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>43831</c:v>
@@ -5709,7 +5709,7 @@
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$61</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>43831</c:v>
@@ -6110,7 +6110,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6258,7 +6258,7 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6414,7 +6414,7 @@
             <c:numRef>
               <c:f>Norway!$A$3:$A$29</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>43190</c:v>
@@ -6630,7 +6630,7 @@
             <c:numRef>
               <c:f>Norway!$A$3:$A$29</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>43190</c:v>
@@ -6851,7 +6851,7 @@
             <c:numRef>
               <c:f>Norway!$A$3:$A$29</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>43190</c:v>
@@ -7054,7 +7054,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -7202,7 +7202,7 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -7348,7 +7348,7 @@
             <c:numRef>
               <c:f>Norway!$A$3:$A$29</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>43190</c:v>
@@ -7564,7 +7564,7 @@
             <c:numRef>
               <c:f>Norway!$A$3:$A$29</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>43190</c:v>
@@ -7785,7 +7785,7 @@
             <c:numRef>
               <c:f>Norway!$A$3:$A$29</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>43190</c:v>
@@ -7988,7 +7988,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -8136,7 +8136,7 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -12112,16 +12112,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDF89A27-C3A9-49F5-AB9A-940148F41631}">
   <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="AC19" sqref="AC19"/>
+    <sheetView topLeftCell="A38" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="348" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="350" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12159,7 +12159,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>43831</v>
       </c>
@@ -12200,7 +12200,7 @@
         <v>2.261247</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>43862</v>
       </c>
@@ -12241,7 +12241,7 @@
         <v>2.3568250000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>43891</v>
       </c>
@@ -12282,7 +12282,7 @@
         <v>2.0913849999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>43922</v>
       </c>
@@ -12323,7 +12323,7 @@
         <v>1.4321550000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>43952</v>
       </c>
@@ -12364,7 +12364,7 @@
         <v>1.2220569999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>43983</v>
       </c>
@@ -12405,7 +12405,7 @@
         <v>1.187414</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>44013</v>
       </c>
@@ -12446,7 +12446,7 @@
         <v>1.569626</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>44044</v>
       </c>
@@ -12487,7 +12487,7 @@
         <v>1.736388</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>44075</v>
       </c>
@@ -12528,7 +12528,7 @@
         <v>1.713279</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>44105</v>
       </c>
@@ -12569,7 +12569,7 @@
         <v>1.6105849999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>44136</v>
       </c>
@@ -12610,7 +12610,7 @@
         <v>1.6464989999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>44166</v>
       </c>
@@ -12651,7 +12651,7 @@
         <v>1.6196429999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>44197</v>
       </c>
@@ -12692,7 +12692,7 @@
         <v>1.410129</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>44228</v>
       </c>
@@ -12733,7 +12733,7 @@
         <v>1.282608</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>44256</v>
       </c>
@@ -12774,7 +12774,7 @@
         <v>1.6463909999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>44287</v>
       </c>
@@ -12815,7 +12815,7 @@
         <v>2.961039</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>44317</v>
       </c>
@@ -12856,7 +12856,7 @@
         <v>3.797606</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>44348</v>
       </c>
@@ -12897,7 +12897,7 @@
         <v>4.4746189999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>44378</v>
       </c>
@@ -12938,7 +12938,7 @@
         <v>4.2745129999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>44409</v>
       </c>
@@ -12979,7 +12979,7 @@
         <v>4.0002829999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>44440</v>
       </c>
@@ -13020,7 +13020,7 @@
         <v>4.0252140000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>44470</v>
       </c>
@@ -13061,7 +13061,7 @@
         <v>4.5628380000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>44501</v>
       </c>
@@ -13102,7 +13102,7 @@
         <v>4.928509</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>44531</v>
       </c>
@@ -13143,7 +13143,7 @@
         <v>5.453411</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>44562</v>
       </c>
@@ -13184,7 +13184,7 @@
         <v>6.0206480000000004</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>44593</v>
       </c>
@@ -13225,7 +13225,7 @@
         <v>6.4142060000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>44621</v>
       </c>
@@ -13266,7 +13266,7 @@
         <v>6.4744789999999997</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>44652</v>
       </c>
@@ -13307,7 +13307,7 @@
         <v>6.1605730000000003</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>44682</v>
       </c>
@@ -13348,7 +13348,7 @@
         <v>6.0215370000000004</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>44713</v>
       </c>
@@ -13389,7 +13389,7 @@
         <v>5.9169429999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>44743</v>
       </c>
@@ -13430,7 +13430,7 @@
         <v>5.9108850000000004</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>44774</v>
       </c>
@@ -13471,7 +13471,7 @@
         <v>6.322203</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>44805</v>
       </c>
@@ -13512,7 +13512,7 @@
         <v>6.6306039999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>44835</v>
       </c>
@@ -13553,7 +13553,7 @@
         <v>6.2844220000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>44866</v>
       </c>
@@ -13594,7 +13594,7 @@
         <v>5.9578290000000003</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>44896</v>
       </c>
@@ -13635,7 +13635,7 @@
         <v>5.7078350000000002</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>44927</v>
       </c>
@@ -13676,7 +13676,7 @@
         <v>5.5825959999999997</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>44958</v>
       </c>
@@ -13717,7 +13717,7 @@
         <v>5.5377539999999996</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>44986</v>
       </c>
@@ -13758,7 +13758,7 @@
         <v>5.5896030000000003</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>45017</v>
       </c>
@@ -13799,7 +13799,7 @@
         <v>5.5194159999999997</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>45047</v>
       </c>
@@ -13840,7 +13840,7 @@
         <v>5.3298050000000003</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>45078</v>
       </c>
@@ -13881,7 +13881,7 @@
         <v>4.8289669999999996</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>45108</v>
       </c>
@@ -13922,7 +13922,7 @@
         <v>4.6528619999999998</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>45139</v>
       </c>
@@ -13963,7 +13963,7 @@
         <v>4.3492449999999998</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>45170</v>
       </c>
@@ -14004,7 +14004,7 @@
         <v>4.1465339999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>45200</v>
       </c>
@@ -14045,7 +14045,7 @@
         <v>4.0308700000000002</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>45231</v>
       </c>
@@ -14086,7 +14086,7 @@
         <v>4.0073429999999997</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>45261</v>
       </c>
@@ -14127,7 +14127,7 @@
         <v>3.929853</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>45292</v>
       </c>
@@ -14168,7 +14168,7 @@
         <v>3.8617439999999998</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>45323</v>
       </c>
@@ -14209,7 +14209,7 @@
         <v>3.7524959999999998</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>45352</v>
       </c>
@@ -14250,7 +14250,7 @@
         <v>3.8012809999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>45383</v>
       </c>
@@ -14291,7 +14291,7 @@
         <v>3.609982</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>45413</v>
       </c>
@@ -14332,7 +14332,7 @@
         <v>3.4187400000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>45444</v>
       </c>
@@ -14373,7 +14373,7 @@
         <v>3.2672949999999998</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>45474</v>
       </c>
@@ -14414,7 +14414,7 @@
         <v>3.1712790000000002</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>45505</v>
       </c>
@@ -14455,7 +14455,7 @@
         <v>3.1970019999999999</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>45536</v>
       </c>
@@ -14496,7 +14496,7 @@
         <v>3.3112729999999999</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>45566</v>
       </c>
@@ -14537,7 +14537,7 @@
         <v>3.3329049999999998</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>45597</v>
       </c>
@@ -14578,7 +14578,7 @@
         <v>3.3186140000000002</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>45627</v>
       </c>
@@ -14629,16 +14629,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D3A8428-ED99-4A0D-A0B5-DB176243C36F}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
         <v>12</v>
@@ -14653,7 +14653,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
         <v>13</v>
@@ -14665,7 +14665,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>43190</v>
       </c>
@@ -14679,7 +14679,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>43281</v>
       </c>
@@ -14693,7 +14693,7 @@
         <v>1.28</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>43373</v>
       </c>
@@ -14707,7 +14707,7 @@
         <v>1.69</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>43465</v>
       </c>
@@ -14721,7 +14721,7 @@
         <v>2.0299999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>43555</v>
       </c>
@@ -14735,7 +14735,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>43646</v>
       </c>
@@ -14749,7 +14749,7 @@
         <v>2.39</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>43738</v>
       </c>
@@ -14763,7 +14763,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>43830</v>
       </c>
@@ -14777,7 +14777,7 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>43921</v>
       </c>
@@ -14791,7 +14791,7 @@
         <v>2.41</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>44012</v>
       </c>
@@ -14805,7 +14805,7 @@
         <v>2.95</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>44104</v>
       </c>
@@ -14819,7 +14819,7 @@
         <v>3.47</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>44196</v>
       </c>
@@ -14833,7 +14833,7 @@
         <v>3.14</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>44286</v>
       </c>
@@ -14847,7 +14847,7 @@
         <v>2.72</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>44377</v>
       </c>
@@ -14861,7 +14861,7 @@
         <v>1.61</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>44469</v>
       </c>
@@ -14875,7 +14875,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>44561</v>
       </c>
@@ -14889,7 +14889,7 @@
         <v>1.36</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>44651</v>
       </c>
@@ -14903,7 +14903,7 @@
         <v>1.88</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
         <v>44742</v>
       </c>
@@ -14917,7 +14917,7 @@
         <v>3.24</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <v>44834</v>
       </c>
@@ -14931,7 +14931,7 @@
         <v>4.84</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
         <v>44926</v>
       </c>
@@ -14945,7 +14945,7 @@
         <v>5.75</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
         <v>45016</v>
       </c>
@@ -14959,7 +14959,7 @@
         <v>6.23</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
         <v>45107</v>
       </c>
@@ -14973,7 +14973,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
         <v>45199</v>
       </c>
@@ -14987,7 +14987,7 @@
         <v>6.04</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <v>45291</v>
       </c>
@@ -15001,7 +15001,7 @@
         <v>5.74</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <v>45382</v>
       </c>
@@ -15015,7 +15015,7 @@
         <v>4.8899999999999997</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
         <v>45473</v>
       </c>
@@ -15029,7 +15029,7 @@
         <v>3.93</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="5">
         <v>45565</v>
       </c>
@@ -15043,7 +15043,7 @@
         <v>3.22</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="5"/>
       <c r="B30" s="7"/>
     </row>

</xml_diff>